<commit_message>
Ghasty_001 animated sprites, credits update
</commit_message>
<xml_diff>
--- a/Créditos_Sprites_Megas ZA_y_DLC_Actualizado.xlsx
+++ b/Créditos_Sprites_Megas ZA_y_DLC_Actualizado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Family\Desktop\Excels_Sprites_Nuevas_Megas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irfan\OneDrive\Documents\GitHub\Pokemon-Essentials-21-With-Unofficial-EBDX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5528E3-2588-460F-A43A-ABCFF3F1FF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C504024-6587-4970-B13A-09D886655B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0DCD06E0-05AA-4A9B-A264-97E2CC42F287}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0DCD06E0-05AA-4A9B-A264-97E2CC42F287}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprites" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="106">
   <si>
     <t>Pokémon (Mega)</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Pokémon</t>
   </si>
   <si>
-    <t>Megapiedra</t>
-  </si>
-  <si>
     <t>Zeraora</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>MizterBubu</t>
   </si>
   <si>
-    <t>MCBMechachu</t>
-  </si>
-  <si>
     <t>flea_alex</t>
   </si>
   <si>
@@ -340,6 +334,15 @@
   </si>
   <si>
     <t>No hay créditos todavía porque no se ha hecho el sprite (ya ninguno)</t>
+  </si>
+  <si>
+    <t>Ghasty_001</t>
+  </si>
+  <si>
+    <t>Ghasty_001, static by kiriaura</t>
+  </si>
+  <si>
+    <t>New sprite; replaces La Base de Sky animated sprite</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,8 +482,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -536,30 +545,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -568,7 +553,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -600,15 +585,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -624,13 +600,19 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="40% - Énfasis3" xfId="4" builtinId="39"/>
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
-    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto explicativo" xfId="3" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,9 +641,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -699,7 +681,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -805,7 +787,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -947,7 +929,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -955,13 +937,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85377A4A-87C9-4718-8F46-84037EE50D6D}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.5546875" bestFit="1" customWidth="1"/>
@@ -970,39 +952,36 @@
     <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="97" customWidth="1"/>
+    <col min="11" max="11" width="97" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="14" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="16" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1013,1288 +992,1147 @@
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>49</v>
+      <c r="B8" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>47</v>
+      <c r="B10" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="B16" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="E37" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E38" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="D40" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="E40" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H43" s="13"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="B48" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="B49" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H49" s="12"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
-        <v>84</v>
-      </c>
       <c r="B50" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H50" s="13"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="H48:H50"/>
+  <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H42:H43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>